<commit_message>
Update - Retrieve files
</commit_message>
<xml_diff>
--- a/DataCollection/AllData_raw_csv/Model7_ParametersRelationshipEquations.xlsx
+++ b/DataCollection/AllData_raw_csv/Model7_ParametersRelationshipEquations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\AllData_raw_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51452BE9-BB9A-4B5F-AE0C-E53709ADFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1971E1D9-5124-4E24-B19C-D2FADC3F9275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAAB5050-1A85-437A-BD70-2C7AA72D08D0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAAB5050-1A85-437A-BD70-2C7AA72D08D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2692,7 +2692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD24BCA-FDA0-4A57-80CB-B8ACE533EEB1}">
   <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>

</xml_diff>